<commit_message>
fixed type at citation sheet
</commit_message>
<xml_diff>
--- a/utils/excel_creator/example_file.xlsx
+++ b/utils/excel_creator/example_file.xlsx
@@ -4949,7 +4949,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5067,6 +5067,13 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>NOMAD Hysprint: NOMAD's schema for HZB perovskite research. NOMAD-HZB contributors. 2025. GitHub. https://github.com/nomad-hzb/nomad-hysprint. Accessed: 2025-04-25. Version: main branch, commit [commit-hash]. Code licensed under Apache-2.0; Voila notebooks licensed under CC BY 4.0.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>

</xml_diff>